<commit_message>
Uploading scripts and outputs for my work to match orthogroups across taxonomic levels based on the sequences they contain.
</commit_message>
<xml_diff>
--- a/Gene_identity.xlsx
+++ b/Gene_identity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="677" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6A55757-67D4-41E4-BBF3-B4EA35862D2C}"/>
+  <xr:revisionPtr revIDLastSave="681" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B57320B1-FDA8-4504-8900-56287C197670}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="732" yWindow="2280" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="300">
   <si>
     <t>Gene</t>
   </si>
@@ -1039,13 +1039,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1351,21 +1352,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="2" width="57.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
-    <col min="6" max="6" width="53.33203125" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>297</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1425,7 +1426,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1666,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1745,7 +1746,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1785,7 +1786,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1825,7 +1826,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1965,7 +1966,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1998,14 +1999,9 @@
       <c r="D32" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -2019,7 +2015,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2033,7 +2029,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2047,7 +2043,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2061,7 +2057,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2075,7 +2071,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2089,7 +2085,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2103,7 +2099,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -2117,7 +2113,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -2131,7 +2127,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -2145,7 +2141,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2159,7 +2155,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2173,7 +2169,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2187,7 +2183,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -2201,7 +2197,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2215,7 +2211,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -2229,7 +2225,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2243,7 +2239,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
@@ -2257,7 +2253,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
@@ -2271,7 +2267,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2285,7 +2281,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
@@ -2299,7 +2295,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2313,7 +2309,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
@@ -2327,7 +2323,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
@@ -2341,7 +2337,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
@@ -2355,7 +2351,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2369,7 +2365,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2383,7 +2379,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
@@ -2397,7 +2393,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
@@ -2411,7 +2407,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
@@ -2425,7 +2421,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
@@ -2439,7 +2435,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
@@ -2453,7 +2449,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2467,7 +2463,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
@@ -2481,7 +2477,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -2495,7 +2491,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2509,7 +2505,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2523,7 +2519,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2537,7 +2533,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -2551,7 +2547,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2565,7 +2561,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2579,7 +2575,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2593,7 +2589,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
@@ -2607,7 +2603,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2621,7 +2617,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2635,7 +2631,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2649,7 +2645,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2663,7 +2659,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2677,7 +2673,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
@@ -2691,7 +2687,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2705,7 +2701,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2719,7 +2715,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2733,7 +2729,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2747,7 +2743,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2761,7 +2757,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -2775,7 +2771,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2789,7 +2785,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2803,7 +2799,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
@@ -2817,7 +2813,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
@@ -2831,7 +2827,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -2845,7 +2841,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2859,7 +2855,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
@@ -2873,7 +2869,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
@@ -2887,7 +2883,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
@@ -2901,7 +2897,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -2915,7 +2911,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
@@ -2929,7 +2925,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
@@ -2943,7 +2939,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
@@ -2957,7 +2953,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -2971,7 +2967,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
@@ -2985,7 +2981,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2999,7 +2995,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -3013,7 +3009,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
@@ -3027,7 +3023,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
@@ -3041,7 +3037,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -3055,7 +3051,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -3069,7 +3065,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -3083,7 +3079,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
@@ -3097,7 +3093,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -3111,7 +3107,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
@@ -3125,7 +3121,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
@@ -3139,7 +3135,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
@@ -3153,7 +3149,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
@@ -3167,7 +3163,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Updates to family level directories to remove data for documents only containing genus level data. I also re-included OG0000030 which was incorrectly excluded from a number of files.
</commit_message>
<xml_diff>
--- a/Gene_identity.xlsx
+++ b/Gene_identity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="681" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B57320B1-FDA8-4504-8900-56287C197670}"/>
+  <xr:revisionPtr revIDLastSave="683" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6400ADD-645A-4279-AF2C-D08C7656C087}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="300">
   <si>
     <t>Gene</t>
   </si>
@@ -1039,14 +1039,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,7 +1352,7 @@
   <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,7 +1998,12 @@
       <c r="D32" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">

</xml_diff>

<commit_message>
Changes related to the inclusion of alignments mistakenly not included in the analysis as part of the alignment processing and gene tree review stages. I also removed alignment files not necessary to include for the family level alignment processing stage.
</commit_message>
<xml_diff>
--- a/Gene_identity.xlsx
+++ b/Gene_identity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6400ADD-645A-4279-AF2C-D08C7656C087}"/>
+  <xr:revisionPtr revIDLastSave="690" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA2E4078-8869-412D-AD07-6608FB8D9704}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="302">
   <si>
     <t>Gene</t>
   </si>
@@ -984,6 +984,12 @@
   </si>
   <si>
     <t>Family Orthogroup</t>
+  </si>
+  <si>
+    <t>OG0000115</t>
+  </si>
+  <si>
+    <t>Nucleoside triphosphate pyrophosphatase</t>
   </si>
 </sst>
 </file>
@@ -1039,13 +1045,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1349,15 +1357,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" workbookViewId="0">
+      <selection activeCell="A76" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="47.7109375" customWidth="1"/>
@@ -1366,7 +1374,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>297</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1386,7 +1394,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1406,7 +1414,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1426,7 +1434,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1446,7 +1454,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1466,7 +1474,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1486,7 +1494,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1506,7 +1514,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1526,7 +1534,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1546,7 +1554,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1566,7 +1574,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1586,7 +1594,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -1606,7 +1614,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1626,7 +1634,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1646,7 +1654,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1666,7 +1674,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1686,7 +1694,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1706,7 +1714,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1726,7 +1734,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1746,7 +1754,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1766,7 +1774,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1786,7 +1794,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1806,7 +1814,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1826,7 +1834,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1846,7 +1854,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1866,7 +1874,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1886,7 +1894,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1906,7 +1914,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1926,7 +1934,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1946,7 +1954,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1966,7 +1974,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1986,7 +1994,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -2006,7 +2014,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2020,7 +2028,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -2034,7 +2042,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2048,7 +2056,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -2062,7 +2070,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -2076,7 +2084,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
@@ -2090,7 +2098,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -2104,7 +2112,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2118,7 +2126,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2132,7 +2140,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -2146,7 +2154,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2160,7 +2168,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
@@ -2174,7 +2182,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
@@ -2188,7 +2196,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2202,7 +2210,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2216,7 +2224,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2230,7 +2238,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
@@ -2244,7 +2252,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2258,7 +2266,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2272,7 +2280,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2286,7 +2294,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -2300,7 +2308,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B54" t="s">
@@ -2314,7 +2322,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -2328,7 +2336,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2342,7 +2350,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2356,7 +2364,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B58" t="s">
@@ -2370,7 +2378,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
@@ -2384,7 +2392,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -2398,7 +2406,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -2412,7 +2420,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2426,7 +2434,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2440,7 +2448,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -2454,7 +2462,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B65" t="s">
@@ -2468,7 +2476,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -2482,7 +2490,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -2496,7 +2504,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B68" t="s">
@@ -2510,7 +2518,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B69" t="s">
@@ -2524,7 +2532,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B70" t="s">
@@ -2538,7 +2546,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -2552,7 +2560,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B72" t="s">
@@ -2566,7 +2574,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B73" t="s">
@@ -2580,7 +2588,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="5" t="s">
         <v>73</v>
       </c>
       <c r="B74" t="s">
@@ -2594,7 +2602,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="5" t="s">
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -2608,7 +2616,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B76" t="s">
@@ -2622,7 +2630,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="s">
@@ -2636,7 +2644,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B78" t="s">
@@ -2650,7 +2658,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -2664,7 +2672,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B80" t="s">
@@ -2678,7 +2686,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="5" t="s">
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -2692,7 +2700,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B82" t="s">
@@ -2706,7 +2714,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="5" t="s">
         <v>82</v>
       </c>
       <c r="B83" t="s">
@@ -2720,7 +2728,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B84" t="s">
@@ -2734,7 +2742,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B85" t="s">
@@ -2748,7 +2756,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B86" t="s">
@@ -2762,7 +2770,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -2776,7 +2784,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B88" t="s">
@@ -2790,7 +2798,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B89" t="s">
@@ -2804,7 +2812,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
@@ -2818,7 +2826,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
@@ -2832,7 +2840,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
@@ -2846,7 +2854,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B93" t="s">
@@ -2860,7 +2868,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
@@ -2874,7 +2882,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -2888,7 +2896,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -2902,7 +2910,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -2916,7 +2924,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="5" t="s">
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
@@ -2930,7 +2938,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -2944,7 +2952,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
@@ -2958,7 +2966,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -2972,7 +2980,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
@@ -2986,7 +2994,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B103" t="s">
@@ -3000,7 +3008,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B104" t="s">
@@ -3014,7 +3022,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
@@ -3028,7 +3036,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
@@ -3042,7 +3050,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
@@ -3056,7 +3064,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
@@ -3070,7 +3078,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -3084,7 +3092,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
@@ -3098,7 +3106,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
@@ -3112,7 +3120,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
@@ -3126,7 +3134,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
@@ -3140,7 +3148,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -3154,7 +3162,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
@@ -3168,7 +3176,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
@@ -3179,6 +3187,20 @@
       </c>
       <c r="D116" s="2" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C117" t="s">
+        <v>300</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating excel spreadsheet to remove informal notes.
</commit_message>
<xml_diff>
--- a/Gene_identity.xlsx
+++ b/Gene_identity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3992D81-8966-4978-ADA1-AADDB4860AB8}"/>
+  <xr:revisionPtr revIDLastSave="726" documentId="11_F25DC773A252ABDACC104814915C4A505BDE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5502DA-196A-433C-B351-32FCB17FB618}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="1785" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Species" sheetId="1" r:id="rId1"/>
@@ -41,37 +41,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={C988EEE1-9781-4ED1-95DF-604518CD0D7C}</author>
-    <author>tc={35AAE0BA-B7DA-4B04-82B9-0DE72B57AD8A}</author>
-    <author>tc={B23E715B-5E1B-4C9A-9B63-356B5D852E1A}</author>
     <author>tc={4DEDCC5D-BA02-4A6A-94C5-7BCD85649702}</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C988EEE1-9781-4ED1-95DF-604518CD0D7C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Red if below if high E value (&gt;1) or low bit score &lt;50. Where there were multiple results I took the one with the highest bit score and lowest e value. If first one was ‘unknown./ uncharacterised protein’ I went for the second one with an identity if it had a bit score &gt;50% and e value less then zero</t>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{35AAE0BA-B7DA-4B04-82B9-0DE72B57AD8A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Red if below if high E value (&gt;1) or low bit score &lt;50. Where there were multiple results I took the one with the highest bit score and lowest e value. If first one was ‘unknown./ uncharacterised protein’ I went for the second one with an identity if it had a bit score &gt;50% and e value less then zero</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="2" shapeId="0" xr:uid="{B23E715B-5E1B-4C9A-9B63-356B5D852E1A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Red if below if high E value (&gt;1) or low bit score &lt;50. Where there were multiple results I took the one with the highest bit score and lowest e value. If first one was ‘unknown./ uncharacterised protein’ I went for the second one with an identity if it had a bit score &gt;50% and e value less then zero</t>
-      </text>
-    </comment>
-    <comment ref="B78" authorId="3" shapeId="0" xr:uid="{4DEDCC5D-BA02-4A6A-94C5-7BCD85649702}">
+    <comment ref="B78" authorId="0" shapeId="0" xr:uid="{4DEDCC5D-BA02-4A6A-94C5-7BCD85649702}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1127,15 +1100,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2025-03-20T05:35:01.68" personId="{E3997474-2DE3-41CA-9B86-8C03481FB0FB}" id="{C988EEE1-9781-4ED1-95DF-604518CD0D7C}">
-    <text>Red if below if high E value (&gt;1) or low bit score &lt;50. Where there were multiple results I took the one with the highest bit score and lowest e value. If first one was ‘unknown./ uncharacterised protein’ I went for the second one with an identity if it had a bit score &gt;50% and e value less then zero</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2025-03-20T05:35:01.68" personId="{E3997474-2DE3-41CA-9B86-8C03481FB0FB}" id="{35AAE0BA-B7DA-4B04-82B9-0DE72B57AD8A}">
-    <text>Red if below if high E value (&gt;1) or low bit score &lt;50. Where there were multiple results I took the one with the highest bit score and lowest e value. If first one was ‘unknown./ uncharacterised protein’ I went for the second one with an identity if it had a bit score &gt;50% and e value less then zero</text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2025-03-20T05:35:01.68" personId="{E3997474-2DE3-41CA-9B86-8C03481FB0FB}" id="{B23E715B-5E1B-4C9A-9B63-356B5D852E1A}">
-    <text>Red if below if high E value (&gt;1) or low bit score &lt;50. Where there were multiple results I took the one with the highest bit score and lowest e value. If first one was ‘unknown./ uncharacterised protein’ I went for the second one with an identity if it had a bit score &gt;50% and e value less then zero</text>
-  </threadedComment>
   <threadedComment ref="B78" dT="2025-03-20T09:11:27.73" personId="{E3997474-2DE3-41CA-9B86-8C03481FB0FB}" id="{4DEDCC5D-BA02-4A6A-94C5-7BCD85649702}">
     <text>A number of hits for S-adenosylmethionine synthase too.</text>
   </threadedComment>
@@ -1147,21 +1111,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>194</v>
       </c>
@@ -1181,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1201,7 +1165,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1221,7 +1185,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1241,7 +1205,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1263,7 +1227,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1283,7 +1247,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1303,7 +1267,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1323,7 +1287,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1343,7 +1307,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1363,7 +1327,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1383,7 +1347,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1403,7 +1367,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1423,7 +1387,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1407,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1463,7 +1427,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1483,7 +1447,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1467,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1523,7 +1487,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1543,7 +1507,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1563,7 +1527,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1583,7 +1547,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1603,7 +1567,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1623,7 +1587,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1643,7 +1607,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1663,7 +1627,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1683,7 +1647,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1703,7 +1667,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1723,7 +1687,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1743,7 +1707,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1763,7 +1727,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1783,7 +1747,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1803,7 +1767,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1817,7 +1781,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1831,7 +1795,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1845,7 +1809,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1859,7 +1823,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1873,7 +1837,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1887,7 +1851,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1901,7 +1865,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1915,7 +1879,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1929,7 +1893,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1943,7 +1907,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1957,7 +1921,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1971,7 +1935,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1985,7 +1949,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1999,7 +1963,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2013,7 +1977,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2027,7 +1991,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2041,7 +2005,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2055,7 +2019,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2069,7 +2033,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2083,7 +2047,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2097,7 +2061,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2111,7 +2075,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2125,7 +2089,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2139,7 +2103,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2153,7 +2117,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2167,7 +2131,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2181,7 +2145,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2195,7 +2159,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2209,7 +2173,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2223,7 +2187,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2237,7 +2201,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2251,7 +2215,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2265,7 +2229,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2279,7 +2243,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2293,7 +2257,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2307,7 +2271,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2321,7 +2285,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2335,7 +2299,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2349,7 +2313,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2363,7 +2327,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2377,7 +2341,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2391,7 +2355,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2405,7 +2369,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2419,7 +2383,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2433,7 +2397,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2447,7 +2411,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2461,7 +2425,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2475,7 +2439,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2489,7 +2453,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2503,7 +2467,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2517,7 +2481,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2531,7 +2495,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2545,7 +2509,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2559,7 +2523,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2573,7 +2537,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2587,7 +2551,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2601,7 +2565,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2615,7 +2579,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2629,7 +2593,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2643,7 +2607,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2657,7 +2621,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2671,7 +2635,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2685,7 +2649,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2699,7 +2663,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2713,7 +2677,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2727,7 +2691,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2741,7 +2705,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2755,7 +2719,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2769,7 +2733,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2783,7 +2747,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2797,7 +2761,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2811,7 +2775,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2825,7 +2789,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2839,7 +2803,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2853,7 +2817,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2867,7 +2831,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2881,7 +2845,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2895,7 +2859,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2909,7 +2873,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2923,7 +2887,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2937,7 +2901,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2951,7 +2915,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2965,7 +2929,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2979,7 +2943,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>197</v>
       </c>

</xml_diff>